<commit_message>
tweaks to differentials and fix broken link
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
+++ b/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
@@ -1940,7 +1940,7 @@
     <t xml:space="preserve">SPOUSEL </t>
   </si>
   <si>
-    <t>name.family, name.use = 'maiden</t>
+    <t>name.family, name.use = maiden</t>
   </si>
   <si>
     <t>Decedent's Residence - Street number</t>
@@ -6292,7 +6292,7 @@
 U = Unknown</t>
   </si>
   <si>
-    <t>ProcedureArtificialInsemination</t>
+    <t>ProcedureFertilityEnhancingDrugTherapyArtificialInsemination</t>
   </si>
   <si>
     <t>Remove Observation-pregnancy-risk-factor</t>
@@ -6307,7 +6307,7 @@
     <t>Y, N, X, U  (BLANK IF NOT ADDED)</t>
   </si>
   <si>
-    <t>ProcedureAssistedFertilization</t>
+    <t>ProcedureAssistedReproductiveTechnology</t>
   </si>
   <si>
     <t>4 digit year; &gt;=year of delivery, Blank (Date of Registration must be a valid date or entirely blank; no portions of the date may be unknown)</t>
@@ -9639,7 +9639,7 @@
   <sheetPr>
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A1:S277"/>
+  <dimension ref="A1:R277"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9656,7 +9656,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -9711,9 +9711,8 @@
       <c r="R1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="3"/>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9756,7 +9755,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9799,7 +9798,7 @@
       </c>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>6</v>
       </c>
@@ -9842,7 +9841,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>6</v>
       </c>
@@ -9882,7 +9881,7 @@
       <c r="N5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>7</v>
       </c>
@@ -9925,7 +9924,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>8</v>
       </c>
@@ -9968,7 +9967,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>9</v>
       </c>
@@ -10011,7 +10010,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>9</v>
       </c>
@@ -10050,7 +10049,7 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>10</v>
       </c>
@@ -10093,7 +10092,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>11</v>
       </c>
@@ -10136,7 +10135,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>12</v>
       </c>
@@ -10179,7 +10178,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>13</v>
       </c>
@@ -10222,7 +10221,7 @@
       </c>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>13</v>
       </c>
@@ -10265,7 +10264,7 @@
       </c>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>14</v>
       </c>
@@ -10306,7 +10305,7 @@
       </c>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>15</v>
       </c>
@@ -21119,7 +21118,7 @@
   <sheetPr>
     <tabColor rgb="FFFF99CC"/>
   </sheetPr>
-  <dimension ref="A1:S46"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -21136,7 +21135,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -21191,9 +21190,8 @@
       <c r="R1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="5"/>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:18">
       <c r="B2">
         <v>1</v>
       </c>
@@ -21230,7 +21228,7 @@
       <c r="N2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -21265,7 +21263,7 @@
       <c r="N3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:18">
       <c r="B4" t="s">
         <v>42</v>
       </c>
@@ -21300,7 +21298,7 @@
       <c r="N4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="B5" t="s">
         <v>42</v>
       </c>
@@ -21335,7 +21333,7 @@
       <c r="N5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:18">
       <c r="B6" t="s">
         <v>42</v>
       </c>
@@ -21372,7 +21370,7 @@
       <c r="N6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:18">
       <c r="B7" t="s">
         <v>946</v>
       </c>
@@ -21409,7 +21407,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:18">
       <c r="B8" t="s">
         <v>42</v>
       </c>
@@ -21446,7 +21444,7 @@
       <c r="N8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:18">
       <c r="B9" t="s">
         <v>42</v>
       </c>
@@ -21483,7 +21481,7 @@
       <c r="N9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:18">
       <c r="B10" t="s">
         <v>42</v>
       </c>
@@ -21520,7 +21518,7 @@
       <c r="N10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:18">
       <c r="B11" t="s">
         <v>42</v>
       </c>
@@ -21557,7 +21555,7 @@
       <c r="N11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:18">
       <c r="B12" t="s">
         <v>42</v>
       </c>
@@ -21594,7 +21592,7 @@
       <c r="N12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>431</v>
       </c>
@@ -21634,7 +21632,7 @@
       <c r="N13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>432</v>
       </c>
@@ -21674,7 +21672,7 @@
       <c r="N14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>433</v>
       </c>
@@ -21714,7 +21712,7 @@
       <c r="N15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>434</v>
       </c>
@@ -22972,7 +22970,7 @@
   <sheetPr>
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A1:S160"/>
+  <dimension ref="A1:R160"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -22989,7 +22987,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -23044,9 +23042,8 @@
       <c r="R1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="3"/>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>272</v>
       </c>
@@ -23089,7 +23086,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>430</v>
       </c>
@@ -23129,7 +23126,7 @@
       <c r="N3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>273</v>
       </c>
@@ -23172,7 +23169,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>275</v>
       </c>
@@ -23215,7 +23212,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>276</v>
       </c>
@@ -23258,7 +23255,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>277</v>
       </c>
@@ -23299,7 +23296,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>278</v>
       </c>
@@ -23340,7 +23337,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>279</v>
       </c>
@@ -23383,7 +23380,7 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>280</v>
       </c>
@@ -23424,7 +23421,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>281</v>
       </c>
@@ -23465,7 +23462,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>282</v>
       </c>
@@ -23508,7 +23505,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>283</v>
       </c>
@@ -23551,7 +23548,7 @@
       </c>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>284</v>
       </c>
@@ -23594,7 +23591,7 @@
       </c>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>285</v>
       </c>
@@ -23637,7 +23634,7 @@
       </c>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>286</v>
       </c>
@@ -29770,7 +29767,7 @@
   <sheetPr>
     <tabColor rgb="FFCC99FF"/>
   </sheetPr>
-  <dimension ref="A1:S160"/>
+  <dimension ref="A1:R160"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -29787,7 +29784,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -29842,9 +29839,8 @@
       <c r="R1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="6"/>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>1183</v>
       </c>
@@ -29877,7 +29873,7 @@
       <c r="N2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>1184</v>
       </c>
@@ -29910,7 +29906,7 @@
       <c r="N3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>1185</v>
       </c>
@@ -29943,7 +29939,7 @@
       <c r="N4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>1186</v>
       </c>
@@ -29976,7 +29972,7 @@
       <c r="N5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>1187</v>
       </c>
@@ -30009,7 +30005,7 @@
       <c r="N6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>1188</v>
       </c>
@@ -30042,7 +30038,7 @@
       <c r="N7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>1189</v>
       </c>
@@ -30075,7 +30071,7 @@
       <c r="N8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>1190</v>
       </c>
@@ -30108,7 +30104,7 @@
       <c r="N9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>1191</v>
       </c>
@@ -30141,7 +30137,7 @@
       <c r="N10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>1192</v>
       </c>
@@ -30174,7 +30170,7 @@
       <c r="N11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>1193</v>
       </c>
@@ -30207,7 +30203,7 @@
       <c r="N12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>1194</v>
       </c>
@@ -30240,7 +30236,7 @@
       <c r="N13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>1195</v>
       </c>
@@ -30273,7 +30269,7 @@
       <c r="N14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>1196</v>
       </c>
@@ -30306,7 +30302,7 @@
       <c r="N15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>1197</v>
       </c>
@@ -35102,7 +35098,7 @@
   <sheetPr>
     <tabColor rgb="FFFFCC99"/>
   </sheetPr>
-  <dimension ref="A1:S370"/>
+  <dimension ref="A1:R370"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -35119,7 +35115,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -35174,9 +35170,8 @@
       <c r="R1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="7"/>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>818</v>
       </c>
@@ -35218,7 +35213,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>819</v>
       </c>
@@ -35260,7 +35255,7 @@
       </c>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>820</v>
       </c>
@@ -35299,7 +35294,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>820</v>
       </c>
@@ -35338,7 +35333,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>820</v>
       </c>
@@ -35377,7 +35372,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>821</v>
       </c>
@@ -35415,7 +35410,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>822</v>
       </c>
@@ -35454,7 +35449,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>822</v>
       </c>
@@ -35493,7 +35488,7 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>822</v>
       </c>
@@ -35532,7 +35527,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>823</v>
       </c>
@@ -35574,7 +35569,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>824</v>
       </c>
@@ -35616,7 +35611,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>825</v>
       </c>
@@ -35658,7 +35653,7 @@
       </c>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>826</v>
       </c>
@@ -35700,7 +35695,7 @@
       </c>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>827</v>
       </c>
@@ -35742,7 +35737,7 @@
       </c>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>828</v>
       </c>
@@ -49875,7 +49870,7 @@
   <sheetPr>
     <tabColor rgb="FFCCFFFF"/>
   </sheetPr>
-  <dimension ref="A1:S368"/>
+  <dimension ref="A1:R368"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -49892,7 +49887,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -49947,9 +49942,8 @@
       <c r="R1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="8"/>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>465</v>
       </c>
@@ -49991,7 +49985,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>466</v>
       </c>
@@ -50033,7 +50027,7 @@
       </c>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>467</v>
       </c>
@@ -50072,7 +50066,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>467</v>
       </c>
@@ -50111,7 +50105,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>467</v>
       </c>
@@ -50150,7 +50144,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>468</v>
       </c>
@@ -50188,7 +50182,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>469</v>
       </c>
@@ -50227,7 +50221,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>469</v>
       </c>
@@ -50266,7 +50260,7 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>469</v>
       </c>
@@ -50305,7 +50299,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -50344,7 +50338,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -50383,7 +50377,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -50422,7 +50416,7 @@
       </c>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -50461,7 +50455,7 @@
       </c>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -50500,7 +50494,7 @@
       </c>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -64828,7 +64822,7 @@
   <sheetPr>
     <tabColor rgb="FFC4BD97"/>
   </sheetPr>
-  <dimension ref="A1:S350"/>
+  <dimension ref="A1:R350"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -64845,7 +64839,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
@@ -64900,9 +64894,8 @@
       <c r="R1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="9"/>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>1342</v>
       </c>
@@ -64929,7 +64922,7 @@
       <c r="N2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>1343</v>
       </c>
@@ -64956,7 +64949,7 @@
       <c r="N3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>1344</v>
       </c>
@@ -64983,7 +64976,7 @@
       <c r="N4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>1345</v>
       </c>
@@ -65010,7 +65003,7 @@
       <c r="N5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>1346</v>
       </c>
@@ -65037,7 +65030,7 @@
       <c r="N6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>1347</v>
       </c>
@@ -65064,7 +65057,7 @@
       <c r="N7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>1348</v>
       </c>
@@ -65091,7 +65084,7 @@
       <c r="N8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>1349</v>
       </c>
@@ -65118,7 +65111,7 @@
       <c r="N9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>1350</v>
       </c>
@@ -65145,7 +65138,7 @@
       <c r="N10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>1351</v>
       </c>
@@ -65172,7 +65165,7 @@
       <c r="N11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>1352</v>
       </c>
@@ -65199,7 +65192,7 @@
       <c r="N12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>1353</v>
       </c>
@@ -65224,7 +65217,7 @@
       <c r="N13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>1354</v>
       </c>
@@ -65249,7 +65242,7 @@
       <c r="N14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>1355</v>
       </c>
@@ -65276,7 +65269,7 @@
       <c r="N15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>1356</v>
       </c>

</xml_diff>

<commit_message>
added a space for consistency
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
+++ b/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12180" uniqueCount="2785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12178" uniqueCount="2785">
   <si>
     <t>This content was derived from the file IJE_File_Layouts_Version_2021_FHIR* and is automatically generated from the source file IJE_File_Layouts_and_FHIR_Mapping_24-06-21.csv.
 The CSV version of the file is used to drive the content of narrative generated for the Vital Records Implementation Guides (VRDR, BFDR, and VRCL).
@@ -2147,7 +2147,7 @@
     <t>DMOMMDN</t>
   </si>
   <si>
-    <t>name.family , name.use=maiden</t>
+    <t>name.family , name.use = maiden</t>
   </si>
   <si>
     <t>Was case Referred to Medical Examiner/Coroner?</t>
@@ -2439,7 +2439,7 @@
     <t>DMAIDEN</t>
   </si>
   <si>
-    <t>name.text , name.use=maiden</t>
+    <t>name.text , name.use = maiden</t>
   </si>
   <si>
     <t>Decedent's Birth Place City - Code</t>
@@ -5893,7 +5893,7 @@
     <t>code</t>
   </si>
   <si>
-    <t>See  [note on missing method of delivery data]</t>
+    <t>[DeliveryRoutesVS] unless unknown, &lt;br /&gt;See  [note on missing method of delivery data]</t>
   </si>
   <si>
     <t>Method of Delivery--Trial of Labor Attempted</t>
@@ -45909,9 +45909,6 @@
       <c r="L270" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="M270" t="s">
-        <v>104</v>
-      </c>
       <c r="N270" s="1" t="s">
         <v>953</v>
       </c>
@@ -45950,9 +45947,6 @@
       </c>
       <c r="L271" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="M271" t="s">
-        <v>104</v>
       </c>
       <c r="N271" s="1" t="s">
         <v>953</v>

</xml_diff>

<commit_message>
updates to dd flagging
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
+++ b/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12797" uniqueCount="2788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12796" uniqueCount="2788">
   <si>
     <t>This content was derived from the file IJE_File_Layouts_Version_2021_FHIR* and is automatically generated from the source file IJE_File_Layouts_and_FHIR_Mapping_24-06-21.csv.
 The CSV version of the file is used to drive the content of narrative generated for the Vital Records Implementation Guides (VRDR, BFDR, and VRCL).
@@ -10629,9 +10629,6 @@
       </c>
       <c r="N22" s="1"/>
       <c r="P22" s="1"/>
-      <c r="S22" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="23" spans="1:19">
       <c r="A23">

</xml_diff>

<commit_message>
regenerate dd with national flaggin updates
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
+++ b/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12835" uniqueCount="2788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12784" uniqueCount="2788">
   <si>
     <t>This content was derived from the file IJE_File_Layouts_Version_2021_FHIR* and is automatically generated from the source file IJE_File_Layouts_and_FHIR_Mapping_24-06-21.csv.
 The CSV version of the file is used to drive the content of narrative generated for the Vital Records Implementation Guides (VRDR, BFDR, and VRCL).
@@ -13701,9 +13701,6 @@
       </c>
       <c r="N91" s="1"/>
       <c r="P91" s="1"/>
-      <c r="S91" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="92" spans="1:19">
       <c r="A92">
@@ -45036,7 +45033,7 @@
       </c>
       <c r="P224" s="1"/>
     </row>
-    <row r="225" spans="1:19">
+    <row r="225" spans="1:16">
       <c r="A225">
         <v>1035</v>
       </c>
@@ -45071,7 +45068,7 @@
       </c>
       <c r="P225" s="1"/>
     </row>
-    <row r="226" spans="1:19">
+    <row r="226" spans="1:16">
       <c r="A226">
         <v>1036</v>
       </c>
@@ -45113,7 +45110,7 @@
       </c>
       <c r="P226" s="1"/>
     </row>
-    <row r="227" spans="1:19">
+    <row r="227" spans="1:16">
       <c r="A227">
         <v>1037</v>
       </c>
@@ -45155,7 +45152,7 @@
       </c>
       <c r="P227" s="1"/>
     </row>
-    <row r="228" spans="1:19">
+    <row r="228" spans="1:16">
       <c r="A228">
         <v>1038</v>
       </c>
@@ -45197,7 +45194,7 @@
       </c>
       <c r="P228" s="1"/>
     </row>
-    <row r="229" spans="1:19">
+    <row r="229" spans="1:16">
       <c r="A229">
         <v>1039</v>
       </c>
@@ -45236,7 +45233,7 @@
       </c>
       <c r="P229" s="1"/>
     </row>
-    <row r="230" spans="1:19">
+    <row r="230" spans="1:16">
       <c r="A230">
         <v>1040</v>
       </c>
@@ -45271,7 +45268,7 @@
       </c>
       <c r="P230" s="1"/>
     </row>
-    <row r="231" spans="1:19">
+    <row r="231" spans="1:16">
       <c r="A231">
         <v>1041</v>
       </c>
@@ -45310,7 +45307,7 @@
       </c>
       <c r="P231" s="1"/>
     </row>
-    <row r="232" spans="1:19">
+    <row r="232" spans="1:16">
       <c r="A232">
         <v>1042</v>
       </c>
@@ -45348,11 +45345,8 @@
         <v>955</v>
       </c>
       <c r="P232" s="1"/>
-      <c r="S232" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="233" spans="1:19">
+    </row>
+    <row r="233" spans="1:16">
       <c r="A233">
         <v>1043</v>
       </c>
@@ -45390,11 +45384,8 @@
         <v>955</v>
       </c>
       <c r="P233" s="1"/>
-      <c r="S233" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="234" spans="1:19">
+    </row>
+    <row r="234" spans="1:16">
       <c r="A234">
         <v>1044</v>
       </c>
@@ -45432,11 +45423,8 @@
         <v>955</v>
       </c>
       <c r="P234" s="1"/>
-      <c r="S234" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="235" spans="1:19">
+    </row>
+    <row r="235" spans="1:16">
       <c r="A235">
         <v>1045</v>
       </c>
@@ -45474,11 +45462,8 @@
         <v>955</v>
       </c>
       <c r="P235" s="1"/>
-      <c r="S235" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="236" spans="1:19">
+    </row>
+    <row r="236" spans="1:16">
       <c r="A236">
         <v>1046</v>
       </c>
@@ -45516,11 +45501,8 @@
         <v>955</v>
       </c>
       <c r="P236" s="1"/>
-      <c r="S236" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="237" spans="1:19">
+    </row>
+    <row r="237" spans="1:16">
       <c r="A237">
         <v>1047</v>
       </c>
@@ -45558,11 +45540,8 @@
         <v>955</v>
       </c>
       <c r="P237" s="1"/>
-      <c r="S237" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="238" spans="1:19">
+    </row>
+    <row r="238" spans="1:16">
       <c r="A238">
         <v>1048</v>
       </c>
@@ -45600,11 +45579,8 @@
         <v>955</v>
       </c>
       <c r="P238" s="1"/>
-      <c r="S238" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="239" spans="1:19">
+    </row>
+    <row r="239" spans="1:16">
       <c r="A239">
         <v>1049</v>
       </c>
@@ -45642,11 +45618,8 @@
         <v>955</v>
       </c>
       <c r="P239" s="1"/>
-      <c r="S239" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="240" spans="1:19">
+    </row>
+    <row r="240" spans="1:16">
       <c r="A240">
         <v>1050</v>
       </c>
@@ -45684,9 +45657,6 @@
         <v>955</v>
       </c>
       <c r="P240" s="1"/>
-      <c r="S240" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="241" spans="1:19">
       <c r="A241">
@@ -45726,9 +45696,6 @@
         <v>955</v>
       </c>
       <c r="P241" s="1"/>
-      <c r="S241" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="242" spans="1:19">
       <c r="A242">
@@ -45771,9 +45738,6 @@
         <v>955</v>
       </c>
       <c r="P242" s="1"/>
-      <c r="S242" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="243" spans="1:19">
       <c r="A243">
@@ -45816,9 +45780,6 @@
         <v>955</v>
       </c>
       <c r="P243" s="1"/>
-      <c r="S243" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="244" spans="1:19">
       <c r="A244">
@@ -46985,7 +46946,7 @@
       </c>
       <c r="P272" s="1"/>
     </row>
-    <row r="273" spans="1:19">
+    <row r="273" spans="1:18">
       <c r="A273">
         <v>1083</v>
       </c>
@@ -47024,7 +46985,7 @@
       </c>
       <c r="P273" s="1"/>
     </row>
-    <row r="274" spans="1:19">
+    <row r="274" spans="1:18">
       <c r="A274">
         <v>1084</v>
       </c>
@@ -47059,7 +47020,7 @@
       </c>
       <c r="P274" s="1"/>
     </row>
-    <row r="275" spans="1:19">
+    <row r="275" spans="1:18">
       <c r="A275">
         <v>1085</v>
       </c>
@@ -47094,7 +47055,7 @@
       </c>
       <c r="P275" s="1"/>
     </row>
-    <row r="276" spans="1:19">
+    <row r="276" spans="1:18">
       <c r="A276">
         <v>1086</v>
       </c>
@@ -47138,7 +47099,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="277" spans="1:19">
+    <row r="277" spans="1:18">
       <c r="A277">
         <v>1087</v>
       </c>
@@ -47171,7 +47132,7 @@
       </c>
       <c r="P277" s="1"/>
     </row>
-    <row r="278" spans="1:19">
+    <row r="278" spans="1:18">
       <c r="A278">
         <v>1088</v>
       </c>
@@ -47215,7 +47176,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="279" spans="1:19">
+    <row r="279" spans="1:18">
       <c r="A279">
         <v>1089</v>
       </c>
@@ -47248,7 +47209,7 @@
       </c>
       <c r="P279" s="1"/>
     </row>
-    <row r="280" spans="1:19">
+    <row r="280" spans="1:18">
       <c r="A280">
         <v>1090</v>
       </c>
@@ -47293,7 +47254,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="281" spans="1:19">
+    <row r="281" spans="1:18">
       <c r="A281">
         <v>1091</v>
       </c>
@@ -47326,7 +47287,7 @@
       </c>
       <c r="P281" s="1"/>
     </row>
-    <row r="282" spans="1:19">
+    <row r="282" spans="1:18">
       <c r="A282">
         <v>1092</v>
       </c>
@@ -47370,7 +47331,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="283" spans="1:19">
+    <row r="283" spans="1:18">
       <c r="A283">
         <v>1093</v>
       </c>
@@ -47403,7 +47364,7 @@
       </c>
       <c r="P283" s="1"/>
     </row>
-    <row r="284" spans="1:19">
+    <row r="284" spans="1:18">
       <c r="A284">
         <v>1094</v>
       </c>
@@ -47444,11 +47405,8 @@
         <v>955</v>
       </c>
       <c r="P284" s="1"/>
-      <c r="S284" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="285" spans="1:19">
+    </row>
+    <row r="285" spans="1:18">
       <c r="A285">
         <v>1095</v>
       </c>
@@ -47489,11 +47447,8 @@
         <v>955</v>
       </c>
       <c r="P285" s="1"/>
-      <c r="S285" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="286" spans="1:19">
+    </row>
+    <row r="286" spans="1:18">
       <c r="A286">
         <v>1096</v>
       </c>
@@ -47534,11 +47489,8 @@
         <v>955</v>
       </c>
       <c r="P286" s="1"/>
-      <c r="S286" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="287" spans="1:19">
+    </row>
+    <row r="287" spans="1:18">
       <c r="A287">
         <v>1097</v>
       </c>
@@ -47579,11 +47531,8 @@
         <v>955</v>
       </c>
       <c r="P287" s="1"/>
-      <c r="S287" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="288" spans="1:19">
+    </row>
+    <row r="288" spans="1:18">
       <c r="A288">
         <v>1098</v>
       </c>
@@ -47624,11 +47573,8 @@
         <v>955</v>
       </c>
       <c r="P288" s="1"/>
-      <c r="S288" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="289" spans="1:19">
+    </row>
+    <row r="289" spans="1:16">
       <c r="A289">
         <v>1099</v>
       </c>
@@ -47669,11 +47615,8 @@
         <v>955</v>
       </c>
       <c r="P289" s="1"/>
-      <c r="S289" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="290" spans="1:19">
+    </row>
+    <row r="290" spans="1:16">
       <c r="A290">
         <v>1100</v>
       </c>
@@ -47715,7 +47658,7 @@
       </c>
       <c r="P290" s="1"/>
     </row>
-    <row r="291" spans="1:19">
+    <row r="291" spans="1:16">
       <c r="A291">
         <v>1101</v>
       </c>
@@ -47757,7 +47700,7 @@
       </c>
       <c r="P291" s="1"/>
     </row>
-    <row r="292" spans="1:19">
+    <row r="292" spans="1:16">
       <c r="A292">
         <v>1102</v>
       </c>
@@ -47799,7 +47742,7 @@
       </c>
       <c r="P292" s="1"/>
     </row>
-    <row r="293" spans="1:19">
+    <row r="293" spans="1:16">
       <c r="A293">
         <v>1103</v>
       </c>
@@ -47841,7 +47784,7 @@
       </c>
       <c r="P293" s="1"/>
     </row>
-    <row r="294" spans="1:19">
+    <row r="294" spans="1:16">
       <c r="A294">
         <v>1104</v>
       </c>
@@ -47883,7 +47826,7 @@
       </c>
       <c r="P294" s="1"/>
     </row>
-    <row r="295" spans="1:19">
+    <row r="295" spans="1:16">
       <c r="A295">
         <v>1105</v>
       </c>
@@ -47925,7 +47868,7 @@
       </c>
       <c r="P295" s="1"/>
     </row>
-    <row r="296" spans="1:19">
+    <row r="296" spans="1:16">
       <c r="A296">
         <v>1106</v>
       </c>
@@ -47964,7 +47907,7 @@
       </c>
       <c r="P296" s="1"/>
     </row>
-    <row r="297" spans="1:19">
+    <row r="297" spans="1:16">
       <c r="A297">
         <v>1107</v>
       </c>
@@ -48003,7 +47946,7 @@
       </c>
       <c r="P297" s="1"/>
     </row>
-    <row r="298" spans="1:19">
+    <row r="298" spans="1:16">
       <c r="A298">
         <v>1108</v>
       </c>
@@ -48042,7 +47985,7 @@
       </c>
       <c r="P298" s="1"/>
     </row>
-    <row r="299" spans="1:19">
+    <row r="299" spans="1:16">
       <c r="A299">
         <v>1109</v>
       </c>
@@ -48081,7 +48024,7 @@
       </c>
       <c r="P299" s="1"/>
     </row>
-    <row r="300" spans="1:19">
+    <row r="300" spans="1:16">
       <c r="A300">
         <v>1110</v>
       </c>
@@ -48120,7 +48063,7 @@
       </c>
       <c r="P300" s="1"/>
     </row>
-    <row r="301" spans="1:19">
+    <row r="301" spans="1:16">
       <c r="A301">
         <v>1111</v>
       </c>
@@ -48159,7 +48102,7 @@
       </c>
       <c r="P301" s="1"/>
     </row>
-    <row r="302" spans="1:19">
+    <row r="302" spans="1:16">
       <c r="A302">
         <v>1112</v>
       </c>
@@ -48198,7 +48141,7 @@
       </c>
       <c r="P302" s="1"/>
     </row>
-    <row r="303" spans="1:19">
+    <row r="303" spans="1:16">
       <c r="A303">
         <v>1113</v>
       </c>
@@ -48237,7 +48180,7 @@
       </c>
       <c r="P303" s="1"/>
     </row>
-    <row r="304" spans="1:19">
+    <row r="304" spans="1:16">
       <c r="A304">
         <v>1114</v>
       </c>
@@ -49575,7 +49518,7 @@
       </c>
       <c r="P336" s="1"/>
     </row>
-    <row r="337" spans="1:19">
+    <row r="337" spans="1:16">
       <c r="A337">
         <v>1147</v>
       </c>
@@ -49617,7 +49560,7 @@
       </c>
       <c r="P337" s="1"/>
     </row>
-    <row r="338" spans="1:19">
+    <row r="338" spans="1:16">
       <c r="A338">
         <v>1148</v>
       </c>
@@ -49652,7 +49595,7 @@
       </c>
       <c r="P338" s="1"/>
     </row>
-    <row r="339" spans="1:19">
+    <row r="339" spans="1:16">
       <c r="A339">
         <v>1149</v>
       </c>
@@ -49694,7 +49637,7 @@
       </c>
       <c r="P339" s="1"/>
     </row>
-    <row r="340" spans="1:19">
+    <row r="340" spans="1:16">
       <c r="A340">
         <v>1150</v>
       </c>
@@ -49736,7 +49679,7 @@
       </c>
       <c r="P340" s="1"/>
     </row>
-    <row r="341" spans="1:19">
+    <row r="341" spans="1:16">
       <c r="A341">
         <v>1151</v>
       </c>
@@ -49771,7 +49714,7 @@
       </c>
       <c r="P341" s="1"/>
     </row>
-    <row r="342" spans="1:19">
+    <row r="342" spans="1:16">
       <c r="A342">
         <v>1152</v>
       </c>
@@ -49806,7 +49749,7 @@
       </c>
       <c r="P342" s="1"/>
     </row>
-    <row r="343" spans="1:19">
+    <row r="343" spans="1:16">
       <c r="A343">
         <v>1153</v>
       </c>
@@ -49841,7 +49784,7 @@
       </c>
       <c r="P343" s="1"/>
     </row>
-    <row r="344" spans="1:19">
+    <row r="344" spans="1:16">
       <c r="A344">
         <v>1154</v>
       </c>
@@ -49876,7 +49819,7 @@
       </c>
       <c r="P344" s="1"/>
     </row>
-    <row r="345" spans="1:19">
+    <row r="345" spans="1:16">
       <c r="A345">
         <v>1155</v>
       </c>
@@ -49911,7 +49854,7 @@
       </c>
       <c r="P345" s="1"/>
     </row>
-    <row r="346" spans="1:19">
+    <row r="346" spans="1:16">
       <c r="A346">
         <v>1156</v>
       </c>
@@ -49950,7 +49893,7 @@
       </c>
       <c r="P346" s="1"/>
     </row>
-    <row r="347" spans="1:19">
+    <row r="347" spans="1:16">
       <c r="A347">
         <v>1157</v>
       </c>
@@ -49988,11 +49931,8 @@
         <v>955</v>
       </c>
       <c r="P347" s="1"/>
-      <c r="S347" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="348" spans="1:19">
+    </row>
+    <row r="348" spans="1:16">
       <c r="A348">
         <v>1158</v>
       </c>
@@ -50030,11 +49970,8 @@
         <v>955</v>
       </c>
       <c r="P348" s="1"/>
-      <c r="S348" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="349" spans="1:19">
+    </row>
+    <row r="349" spans="1:16">
       <c r="A349">
         <v>1159</v>
       </c>
@@ -50075,11 +50012,8 @@
         <v>955</v>
       </c>
       <c r="P349" s="1"/>
-      <c r="S349" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="350" spans="1:19">
+    </row>
+    <row r="350" spans="1:16">
       <c r="A350">
         <v>1160</v>
       </c>
@@ -50112,7 +50046,7 @@
       </c>
       <c r="P350" s="1"/>
     </row>
-    <row r="351" spans="1:19">
+    <row r="351" spans="1:16">
       <c r="A351">
         <v>1161</v>
       </c>
@@ -50145,7 +50079,7 @@
       </c>
       <c r="P351" s="1"/>
     </row>
-    <row r="352" spans="1:19">
+    <row r="352" spans="1:16">
       <c r="A352">
         <v>1162</v>
       </c>
@@ -50258,9 +50192,6 @@
         <v>955</v>
       </c>
       <c r="P354" s="1"/>
-      <c r="S354" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="355" spans="1:19">
       <c r="A355">
@@ -50303,9 +50234,6 @@
         <v>955</v>
       </c>
       <c r="P355" s="1"/>
-      <c r="S355" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="356" spans="1:19">
       <c r="A356">
@@ -50348,9 +50276,6 @@
         <v>955</v>
       </c>
       <c r="P356" s="1"/>
-      <c r="S356" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="357" spans="1:19">
       <c r="A357">
@@ -62619,9 +62544,6 @@
         <v>955</v>
       </c>
       <c r="P267" s="1"/>
-      <c r="S267" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="268" spans="1:19">
       <c r="A268">
@@ -62661,9 +62583,6 @@
         <v>955</v>
       </c>
       <c r="P268" s="1"/>
-      <c r="S268" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="269" spans="1:19">
       <c r="A269">
@@ -64112,7 +64031,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="305" spans="1:19">
+    <row r="305" spans="1:16">
       <c r="A305">
         <v>753</v>
       </c>
@@ -64147,7 +64066,7 @@
       </c>
       <c r="P305" s="1"/>
     </row>
-    <row r="306" spans="1:19">
+    <row r="306" spans="1:16">
       <c r="A306">
         <v>754</v>
       </c>
@@ -64188,11 +64107,8 @@
         <v>955</v>
       </c>
       <c r="P306" s="1"/>
-      <c r="S306" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="307" spans="1:19">
+    </row>
+    <row r="307" spans="1:16">
       <c r="A307">
         <v>755</v>
       </c>
@@ -64233,11 +64149,8 @@
         <v>955</v>
       </c>
       <c r="P307" s="1"/>
-      <c r="S307" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="308" spans="1:19">
+    </row>
+    <row r="308" spans="1:16">
       <c r="A308">
         <v>756</v>
       </c>
@@ -64279,7 +64192,7 @@
       </c>
       <c r="P308" s="1"/>
     </row>
-    <row r="309" spans="1:19">
+    <row r="309" spans="1:16">
       <c r="A309">
         <v>757</v>
       </c>
@@ -64321,7 +64234,7 @@
       </c>
       <c r="P309" s="1"/>
     </row>
-    <row r="310" spans="1:19">
+    <row r="310" spans="1:16">
       <c r="A310">
         <v>758</v>
       </c>
@@ -64356,7 +64269,7 @@
       </c>
       <c r="P310" s="1"/>
     </row>
-    <row r="311" spans="1:19">
+    <row r="311" spans="1:16">
       <c r="A311">
         <v>759</v>
       </c>
@@ -64398,7 +64311,7 @@
       </c>
       <c r="P311" s="1"/>
     </row>
-    <row r="312" spans="1:19">
+    <row r="312" spans="1:16">
       <c r="A312">
         <v>760</v>
       </c>
@@ -64440,7 +64353,7 @@
       </c>
       <c r="P312" s="1"/>
     </row>
-    <row r="313" spans="1:19">
+    <row r="313" spans="1:16">
       <c r="A313">
         <v>761</v>
       </c>
@@ -64475,7 +64388,7 @@
       </c>
       <c r="P313" s="1"/>
     </row>
-    <row r="314" spans="1:19">
+    <row r="314" spans="1:16">
       <c r="A314">
         <v>762</v>
       </c>
@@ -64510,7 +64423,7 @@
       </c>
       <c r="P314" s="1"/>
     </row>
-    <row r="315" spans="1:19">
+    <row r="315" spans="1:16">
       <c r="A315">
         <v>763</v>
       </c>
@@ -64545,7 +64458,7 @@
       </c>
       <c r="P315" s="1"/>
     </row>
-    <row r="316" spans="1:19">
+    <row r="316" spans="1:16">
       <c r="A316">
         <v>764</v>
       </c>
@@ -64580,7 +64493,7 @@
       </c>
       <c r="P316" s="1"/>
     </row>
-    <row r="317" spans="1:19">
+    <row r="317" spans="1:16">
       <c r="A317">
         <v>765</v>
       </c>
@@ -64615,7 +64528,7 @@
       </c>
       <c r="P317" s="1"/>
     </row>
-    <row r="318" spans="1:19">
+    <row r="318" spans="1:16">
       <c r="A318">
         <v>766</v>
       </c>
@@ -64654,7 +64567,7 @@
       </c>
       <c r="P318" s="1"/>
     </row>
-    <row r="319" spans="1:19">
+    <row r="319" spans="1:16">
       <c r="A319">
         <v>767</v>
       </c>
@@ -64693,7 +64606,7 @@
       </c>
       <c r="P319" s="1"/>
     </row>
-    <row r="320" spans="1:19">
+    <row r="320" spans="1:16">
       <c r="A320">
         <v>768</v>
       </c>
@@ -64732,7 +64645,7 @@
       </c>
       <c r="P320" s="1"/>
     </row>
-    <row r="321" spans="1:19">
+    <row r="321" spans="1:16">
       <c r="A321">
         <v>769</v>
       </c>
@@ -64773,11 +64686,8 @@
         <v>955</v>
       </c>
       <c r="P321" s="1"/>
-      <c r="S321" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="322" spans="1:19">
+    </row>
+    <row r="322" spans="1:16">
       <c r="A322">
         <v>770</v>
       </c>
@@ -64818,11 +64728,8 @@
         <v>955</v>
       </c>
       <c r="P322" s="1"/>
-      <c r="S322" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="323" spans="1:19">
+    </row>
+    <row r="323" spans="1:16">
       <c r="A323">
         <v>771</v>
       </c>
@@ -64863,11 +64770,8 @@
         <v>955</v>
       </c>
       <c r="P323" s="1"/>
-      <c r="S323" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="324" spans="1:19">
+    </row>
+    <row r="324" spans="1:16">
       <c r="A324">
         <v>772</v>
       </c>
@@ -64908,11 +64812,8 @@
         <v>955</v>
       </c>
       <c r="P324" s="1"/>
-      <c r="S324" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="325" spans="1:19">
+    </row>
+    <row r="325" spans="1:16">
       <c r="A325">
         <v>773</v>
       </c>
@@ -64950,11 +64851,8 @@
         <v>955</v>
       </c>
       <c r="P325" s="1"/>
-      <c r="S325" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="326" spans="1:19">
+    </row>
+    <row r="326" spans="1:16">
       <c r="A326">
         <v>774</v>
       </c>
@@ -64992,11 +64890,8 @@
         <v>955</v>
       </c>
       <c r="P326" s="1"/>
-      <c r="S326" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="327" spans="1:19">
+    </row>
+    <row r="327" spans="1:16">
       <c r="A327">
         <v>775</v>
       </c>
@@ -65034,11 +64929,8 @@
         <v>955</v>
       </c>
       <c r="P327" s="1"/>
-      <c r="S327" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="328" spans="1:19">
+    </row>
+    <row r="328" spans="1:16">
       <c r="A328">
         <v>776</v>
       </c>
@@ -65076,11 +64968,8 @@
         <v>955</v>
       </c>
       <c r="P328" s="1"/>
-      <c r="S328" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="329" spans="1:19">
+    </row>
+    <row r="329" spans="1:16">
       <c r="A329">
         <v>777</v>
       </c>
@@ -65118,11 +65007,8 @@
         <v>955</v>
       </c>
       <c r="P329" s="1"/>
-      <c r="S329" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="330" spans="1:19">
+    </row>
+    <row r="330" spans="1:16">
       <c r="A330">
         <v>778</v>
       </c>
@@ -65160,11 +65046,8 @@
         <v>955</v>
       </c>
       <c r="P330" s="1"/>
-      <c r="S330" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="331" spans="1:19">
+    </row>
+    <row r="331" spans="1:16">
       <c r="A331">
         <v>779</v>
       </c>
@@ -65202,11 +65085,8 @@
         <v>955</v>
       </c>
       <c r="P331" s="1"/>
-      <c r="S331" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="332" spans="1:19">
+    </row>
+    <row r="332" spans="1:16">
       <c r="A332">
         <v>780</v>
       </c>
@@ -65244,11 +65124,8 @@
         <v>955</v>
       </c>
       <c r="P332" s="1"/>
-      <c r="S332" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="333" spans="1:19">
+    </row>
+    <row r="333" spans="1:16">
       <c r="A333">
         <v>781</v>
       </c>
@@ -65286,11 +65163,8 @@
         <v>955</v>
       </c>
       <c r="P333" s="1"/>
-      <c r="S333" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="334" spans="1:19">
+    </row>
+    <row r="334" spans="1:16">
       <c r="A334">
         <v>782</v>
       </c>
@@ -65328,11 +65202,8 @@
         <v>955</v>
       </c>
       <c r="P334" s="1"/>
-      <c r="S334" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="335" spans="1:19">
+    </row>
+    <row r="335" spans="1:16">
       <c r="A335">
         <v>783</v>
       </c>
@@ -65373,11 +65244,8 @@
         <v>955</v>
       </c>
       <c r="P335" s="1"/>
-      <c r="S335" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="336" spans="1:19">
+    </row>
+    <row r="336" spans="1:16">
       <c r="A336">
         <v>784</v>
       </c>
@@ -65418,11 +65286,8 @@
         <v>955</v>
       </c>
       <c r="P336" s="1"/>
-      <c r="S336" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="337" spans="1:19">
+    </row>
+    <row r="337" spans="1:16">
       <c r="A337">
         <v>785</v>
       </c>
@@ -65461,7 +65326,7 @@
       </c>
       <c r="P337" s="1"/>
     </row>
-    <row r="338" spans="1:19">
+    <row r="338" spans="1:16">
       <c r="A338">
         <v>786</v>
       </c>
@@ -65496,7 +65361,7 @@
       </c>
       <c r="P338" s="1"/>
     </row>
-    <row r="339" spans="1:19">
+    <row r="339" spans="1:16">
       <c r="A339">
         <v>787</v>
       </c>
@@ -65531,7 +65396,7 @@
       </c>
       <c r="P339" s="1"/>
     </row>
-    <row r="340" spans="1:19">
+    <row r="340" spans="1:16">
       <c r="A340">
         <v>788</v>
       </c>
@@ -65566,7 +65431,7 @@
       </c>
       <c r="P340" s="1"/>
     </row>
-    <row r="341" spans="1:19">
+    <row r="341" spans="1:16">
       <c r="A341">
         <v>789</v>
       </c>
@@ -65601,7 +65466,7 @@
       </c>
       <c r="P341" s="1"/>
     </row>
-    <row r="342" spans="1:19">
+    <row r="342" spans="1:16">
       <c r="A342">
         <v>790</v>
       </c>
@@ -65639,11 +65504,8 @@
         <v>955</v>
       </c>
       <c r="P342" s="1"/>
-      <c r="S342" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="343" spans="1:19">
+    </row>
+    <row r="343" spans="1:16">
       <c r="A343">
         <v>791</v>
       </c>
@@ -65681,11 +65543,8 @@
         <v>955</v>
       </c>
       <c r="P343" s="1"/>
-      <c r="S343" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="344" spans="1:19">
+    </row>
+    <row r="344" spans="1:16">
       <c r="A344">
         <v>792</v>
       </c>
@@ -65723,11 +65582,8 @@
         <v>955</v>
       </c>
       <c r="P344" s="1"/>
-      <c r="S344" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="345" spans="1:19">
+    </row>
+    <row r="345" spans="1:16">
       <c r="A345">
         <v>793</v>
       </c>
@@ -65765,11 +65621,8 @@
         <v>955</v>
       </c>
       <c r="P345" s="1"/>
-      <c r="S345" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="346" spans="1:19">
+    </row>
+    <row r="346" spans="1:16">
       <c r="A346">
         <v>794</v>
       </c>
@@ -65810,11 +65663,8 @@
         <v>955</v>
       </c>
       <c r="P346" s="1"/>
-      <c r="S346" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="347" spans="1:19">
+    </row>
+    <row r="347" spans="1:16">
       <c r="A347">
         <v>795</v>
       </c>
@@ -65852,11 +65702,8 @@
         <v>955</v>
       </c>
       <c r="P347" s="1"/>
-      <c r="S347" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="348" spans="1:19">
+    </row>
+    <row r="348" spans="1:16">
       <c r="A348">
         <v>796</v>
       </c>
@@ -65895,7 +65742,7 @@
       </c>
       <c r="P348" s="1"/>
     </row>
-    <row r="349" spans="1:19">
+    <row r="349" spans="1:16">
       <c r="A349">
         <v>797</v>
       </c>
@@ -65934,7 +65781,7 @@
       </c>
       <c r="P349" s="1"/>
     </row>
-    <row r="350" spans="1:19">
+    <row r="350" spans="1:16">
       <c r="A350">
         <v>798</v>
       </c>
@@ -65976,7 +65823,7 @@
       </c>
       <c r="P350" s="1"/>
     </row>
-    <row r="351" spans="1:19">
+    <row r="351" spans="1:16">
       <c r="A351">
         <v>799</v>
       </c>
@@ -66018,7 +65865,7 @@
       </c>
       <c r="P351" s="1"/>
     </row>
-    <row r="352" spans="1:19">
+    <row r="352" spans="1:16">
       <c r="A352">
         <v>800</v>
       </c>

</xml_diff>